<commit_message>
add dependency and update it automatically on load
</commit_message>
<xml_diff>
--- a/tools/anssi/anssi-guide-hygiene-detail.xlsx
+++ b/tools/anssi/anssi-guide-hygiene-detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/anssi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DC2078-F0B4-3A4A-9947-77E2D878DF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C9B573-5E06-0141-879B-B6EA04EC9250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="35060" windowHeight="20580" activeTab="1" xr2:uid="{125C4C37-F3C0-444B-A950-381456F8AB10}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="35060" windowHeight="20580" xr2:uid="{125C4C37-F3C0-444B-A950-381456F8AB10}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="570">
   <si>
     <t>Sensibiliser et former</t>
   </si>
@@ -1899,6 +1899,12 @@
   </si>
   <si>
     <t xml:space="preserve">• les utilisateurs utilisant un poste non administré par le service informatique et qui ne fait pas l’objet de mesures de sécurité édictées par la politique de sécurité générale de l’entité. </t>
+  </si>
+  <si>
+    <t>library_dependencies</t>
+  </si>
+  <si>
+    <t>urn:intuitem:risk:library:doc-pol</t>
   </si>
 </sst>
 </file>
@@ -1977,7 +1983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2039,9 +2045,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2380,10 +2383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58679FA1-8C3E-D64B-9B35-083A1517BC84}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" zoomScale="242" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="242" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2466,45 +2469,42 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>568</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>110</v>
+        <v>569</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2512,31 +2512,42 @@
         <v>79</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>415</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2547,7 +2558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F3B91E-FB51-FE47-B7BA-EB94A985CF95}">
   <dimension ref="A1:I260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
     </sheetView>
@@ -2651,7 +2662,7 @@
       <c r="C5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>509</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -2671,7 +2682,7 @@
       <c r="C6" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>510</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -2691,7 +2702,7 @@
       <c r="C7" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>511</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -2711,7 +2722,7 @@
       <c r="C8" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>512</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -2731,7 +2742,7 @@
       <c r="C9" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>513</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -2751,7 +2762,7 @@
       <c r="C10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="22" t="s">
         <v>514</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -2771,7 +2782,7 @@
       <c r="C11" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>515</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -2884,7 +2895,7 @@
       <c r="C17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="22" t="s">
         <v>516</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -2904,7 +2915,7 @@
       <c r="C18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="22" t="s">
         <v>517</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -2924,7 +2935,7 @@
       <c r="C19" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="22" t="s">
         <v>518</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -2944,7 +2955,7 @@
       <c r="C20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="22" t="s">
         <v>519</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -2964,7 +2975,7 @@
       <c r="C21" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="22" t="s">
         <v>520</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -3053,7 +3064,7 @@
       <c r="C26" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="22" t="s">
         <v>521</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -3073,7 +3084,7 @@
       <c r="C27" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="22" t="s">
         <v>522</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -3279,7 +3290,7 @@
       <c r="C38" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F38" s="23" t="s">
+      <c r="F38" s="22" t="s">
         <v>523</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -3299,7 +3310,7 @@
       <c r="C39" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F39" s="22" t="s">
         <v>524</v>
       </c>
       <c r="G39" s="4" t="s">
@@ -3319,7 +3330,7 @@
       <c r="C40" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="22" t="s">
         <v>567</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -3412,7 +3423,7 @@
       <c r="C45" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="23" t="s">
+      <c r="F45" s="22" t="s">
         <v>525</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -3432,7 +3443,7 @@
       <c r="C46" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F46" s="23" t="s">
+      <c r="F46" s="22" t="s">
         <v>526</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -3452,7 +3463,7 @@
       <c r="C47" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="22" t="s">
         <v>527</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -3472,7 +3483,7 @@
       <c r="C48" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F48" s="23" t="s">
+      <c r="F48" s="22" t="s">
         <v>528</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -3757,7 +3768,7 @@
       <c r="C63" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F63" s="23" t="s">
+      <c r="F63" s="22" t="s">
         <v>529</v>
       </c>
       <c r="G63" s="4" t="s">
@@ -3777,7 +3788,7 @@
       <c r="C64" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F64" s="23" t="s">
+      <c r="F64" s="22" t="s">
         <v>530</v>
       </c>
       <c r="G64" s="4" t="s">
@@ -3797,7 +3808,7 @@
       <c r="C65" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F65" s="23" t="s">
+      <c r="F65" s="22" t="s">
         <v>531</v>
       </c>
       <c r="G65" s="4" t="s">
@@ -3936,7 +3947,7 @@
       <c r="C72" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F72" s="23" t="s">
+      <c r="F72" s="22" t="s">
         <v>532</v>
       </c>
       <c r="G72" s="4" t="s">
@@ -3956,7 +3967,7 @@
       <c r="C73" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F73" s="23" t="s">
+      <c r="F73" s="22" t="s">
         <v>533</v>
       </c>
       <c r="G73" s="4" t="s">
@@ -3976,7 +3987,7 @@
       <c r="C74" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F74" s="23" t="s">
+      <c r="F74" s="22" t="s">
         <v>534</v>
       </c>
       <c r="G74" s="4" t="s">
@@ -4769,7 +4780,7 @@
       <c r="F114" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="G114" s="22" t="s">
+      <c r="G114" s="4" t="s">
         <v>486</v>
       </c>
       <c r="H114" s="5" t="s">
@@ -4808,7 +4819,7 @@
       <c r="F116" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="G116" s="22" t="s">
+      <c r="G116" s="4" t="s">
         <v>502</v>
       </c>
       <c r="H116" s="4" t="s">
@@ -4831,7 +4842,7 @@
       <c r="F117" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="G117" s="22" t="s">
+      <c r="G117" s="4" t="s">
         <v>487</v>
       </c>
       <c r="I117" s="4" t="s">
@@ -5130,7 +5141,7 @@
       <c r="F132" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="G132" s="22" t="s">
+      <c r="G132" s="4" t="s">
         <v>469</v>
       </c>
       <c r="H132" s="4" t="s">
@@ -5150,7 +5161,7 @@
       <c r="F133" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="G133" s="22" t="s">
+      <c r="G133" s="4" t="s">
         <v>500</v>
       </c>
       <c r="H133" s="4" t="s">
@@ -5173,7 +5184,7 @@
       <c r="F134" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="G134" s="22" t="s">
+      <c r="G134" s="4" t="s">
         <v>501</v>
       </c>
       <c r="H134" s="4" t="s">
@@ -5373,7 +5384,7 @@
       <c r="F144" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="G144" s="22" t="s">
+      <c r="G144" s="4" t="s">
         <v>441</v>
       </c>
       <c r="H144" s="5" t="s">
@@ -5475,7 +5486,7 @@
       <c r="F149" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="G149" s="22" t="s">
+      <c r="G149" s="4" t="s">
         <v>489</v>
       </c>
       <c r="H149" s="5" t="s">
@@ -5698,7 +5709,7 @@
       <c r="F161" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="G161" s="22" t="s">
+      <c r="G161" s="4" t="s">
         <v>507</v>
       </c>
       <c r="H161" s="4" t="s">
@@ -5721,7 +5732,7 @@
       <c r="F162" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="G162" s="22" t="s">
+      <c r="G162" s="4" t="s">
         <v>444</v>
       </c>
       <c r="H162" s="4" t="s">
@@ -5744,7 +5755,7 @@
       <c r="F163" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="G163" s="22" t="s">
+      <c r="G163" s="4" t="s">
         <v>444</v>
       </c>
       <c r="H163" s="4" t="s">
@@ -5767,7 +5778,7 @@
       <c r="F164" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G164" s="22" t="s">
+      <c r="G164" s="4" t="s">
         <v>444</v>
       </c>
       <c r="H164" s="5" t="s">
@@ -6619,7 +6630,7 @@
       <c r="F210" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="G210" s="22" t="s">
+      <c r="G210" s="4" t="s">
         <v>471</v>
       </c>
       <c r="I210" s="5" t="s">

</xml_diff>

<commit_message>
add dependency and update it automatically on load (#1159)
</commit_message>
<xml_diff>
--- a/tools/anssi/anssi-guide-hygiene-detail.xlsx
+++ b/tools/anssi/anssi-guide-hygiene-detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/anssi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DC2078-F0B4-3A4A-9947-77E2D878DF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C9B573-5E06-0141-879B-B6EA04EC9250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="35060" windowHeight="20580" activeTab="1" xr2:uid="{125C4C37-F3C0-444B-A950-381456F8AB10}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="35060" windowHeight="20580" xr2:uid="{125C4C37-F3C0-444B-A950-381456F8AB10}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="570">
   <si>
     <t>Sensibiliser et former</t>
   </si>
@@ -1899,6 +1899,12 @@
   </si>
   <si>
     <t xml:space="preserve">• les utilisateurs utilisant un poste non administré par le service informatique et qui ne fait pas l’objet de mesures de sécurité édictées par la politique de sécurité générale de l’entité. </t>
+  </si>
+  <si>
+    <t>library_dependencies</t>
+  </si>
+  <si>
+    <t>urn:intuitem:risk:library:doc-pol</t>
   </si>
 </sst>
 </file>
@@ -1977,7 +1983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2039,9 +2045,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2380,10 +2383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58679FA1-8C3E-D64B-9B35-083A1517BC84}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" zoomScale="242" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="242" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2466,45 +2469,42 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>568</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>110</v>
+        <v>569</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2512,31 +2512,42 @@
         <v>79</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>415</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2547,7 +2558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F3B91E-FB51-FE47-B7BA-EB94A985CF95}">
   <dimension ref="A1:I260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
     </sheetView>
@@ -2651,7 +2662,7 @@
       <c r="C5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>509</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -2671,7 +2682,7 @@
       <c r="C6" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>510</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -2691,7 +2702,7 @@
       <c r="C7" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>511</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -2711,7 +2722,7 @@
       <c r="C8" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>512</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -2731,7 +2742,7 @@
       <c r="C9" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>513</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -2751,7 +2762,7 @@
       <c r="C10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="22" t="s">
         <v>514</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -2771,7 +2782,7 @@
       <c r="C11" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>515</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -2884,7 +2895,7 @@
       <c r="C17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="22" t="s">
         <v>516</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -2904,7 +2915,7 @@
       <c r="C18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="22" t="s">
         <v>517</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -2924,7 +2935,7 @@
       <c r="C19" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="22" t="s">
         <v>518</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -2944,7 +2955,7 @@
       <c r="C20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="22" t="s">
         <v>519</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -2964,7 +2975,7 @@
       <c r="C21" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="22" t="s">
         <v>520</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -3053,7 +3064,7 @@
       <c r="C26" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="22" t="s">
         <v>521</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -3073,7 +3084,7 @@
       <c r="C27" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="22" t="s">
         <v>522</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -3279,7 +3290,7 @@
       <c r="C38" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F38" s="23" t="s">
+      <c r="F38" s="22" t="s">
         <v>523</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -3299,7 +3310,7 @@
       <c r="C39" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F39" s="22" t="s">
         <v>524</v>
       </c>
       <c r="G39" s="4" t="s">
@@ -3319,7 +3330,7 @@
       <c r="C40" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="22" t="s">
         <v>567</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -3412,7 +3423,7 @@
       <c r="C45" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="23" t="s">
+      <c r="F45" s="22" t="s">
         <v>525</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -3432,7 +3443,7 @@
       <c r="C46" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F46" s="23" t="s">
+      <c r="F46" s="22" t="s">
         <v>526</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -3452,7 +3463,7 @@
       <c r="C47" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="22" t="s">
         <v>527</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -3472,7 +3483,7 @@
       <c r="C48" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F48" s="23" t="s">
+      <c r="F48" s="22" t="s">
         <v>528</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -3757,7 +3768,7 @@
       <c r="C63" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F63" s="23" t="s">
+      <c r="F63" s="22" t="s">
         <v>529</v>
       </c>
       <c r="G63" s="4" t="s">
@@ -3777,7 +3788,7 @@
       <c r="C64" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F64" s="23" t="s">
+      <c r="F64" s="22" t="s">
         <v>530</v>
       </c>
       <c r="G64" s="4" t="s">
@@ -3797,7 +3808,7 @@
       <c r="C65" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F65" s="23" t="s">
+      <c r="F65" s="22" t="s">
         <v>531</v>
       </c>
       <c r="G65" s="4" t="s">
@@ -3936,7 +3947,7 @@
       <c r="C72" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F72" s="23" t="s">
+      <c r="F72" s="22" t="s">
         <v>532</v>
       </c>
       <c r="G72" s="4" t="s">
@@ -3956,7 +3967,7 @@
       <c r="C73" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F73" s="23" t="s">
+      <c r="F73" s="22" t="s">
         <v>533</v>
       </c>
       <c r="G73" s="4" t="s">
@@ -3976,7 +3987,7 @@
       <c r="C74" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F74" s="23" t="s">
+      <c r="F74" s="22" t="s">
         <v>534</v>
       </c>
       <c r="G74" s="4" t="s">
@@ -4769,7 +4780,7 @@
       <c r="F114" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="G114" s="22" t="s">
+      <c r="G114" s="4" t="s">
         <v>486</v>
       </c>
       <c r="H114" s="5" t="s">
@@ -4808,7 +4819,7 @@
       <c r="F116" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="G116" s="22" t="s">
+      <c r="G116" s="4" t="s">
         <v>502</v>
       </c>
       <c r="H116" s="4" t="s">
@@ -4831,7 +4842,7 @@
       <c r="F117" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="G117" s="22" t="s">
+      <c r="G117" s="4" t="s">
         <v>487</v>
       </c>
       <c r="I117" s="4" t="s">
@@ -5130,7 +5141,7 @@
       <c r="F132" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="G132" s="22" t="s">
+      <c r="G132" s="4" t="s">
         <v>469</v>
       </c>
       <c r="H132" s="4" t="s">
@@ -5150,7 +5161,7 @@
       <c r="F133" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="G133" s="22" t="s">
+      <c r="G133" s="4" t="s">
         <v>500</v>
       </c>
       <c r="H133" s="4" t="s">
@@ -5173,7 +5184,7 @@
       <c r="F134" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="G134" s="22" t="s">
+      <c r="G134" s="4" t="s">
         <v>501</v>
       </c>
       <c r="H134" s="4" t="s">
@@ -5373,7 +5384,7 @@
       <c r="F144" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="G144" s="22" t="s">
+      <c r="G144" s="4" t="s">
         <v>441</v>
       </c>
       <c r="H144" s="5" t="s">
@@ -5475,7 +5486,7 @@
       <c r="F149" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="G149" s="22" t="s">
+      <c r="G149" s="4" t="s">
         <v>489</v>
       </c>
       <c r="H149" s="5" t="s">
@@ -5698,7 +5709,7 @@
       <c r="F161" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="G161" s="22" t="s">
+      <c r="G161" s="4" t="s">
         <v>507</v>
       </c>
       <c r="H161" s="4" t="s">
@@ -5721,7 +5732,7 @@
       <c r="F162" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="G162" s="22" t="s">
+      <c r="G162" s="4" t="s">
         <v>444</v>
       </c>
       <c r="H162" s="4" t="s">
@@ -5744,7 +5755,7 @@
       <c r="F163" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="G163" s="22" t="s">
+      <c r="G163" s="4" t="s">
         <v>444</v>
       </c>
       <c r="H163" s="4" t="s">
@@ -5767,7 +5778,7 @@
       <c r="F164" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G164" s="22" t="s">
+      <c r="G164" s="4" t="s">
         <v>444</v>
       </c>
       <c r="H164" s="5" t="s">
@@ -6619,7 +6630,7 @@
       <c r="F210" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="G210" s="22" t="s">
+      <c r="G210" s="4" t="s">
         <v>471</v>
       </c>
       <c r="I210" s="5" t="s">

</xml_diff>

<commit_message>
fix: eager set cast of possibly None implementation_groups field (#1410)
* Fix eager set cast of possibly None implementation_groups field

* fix missing IG

this was causing the issue with null set

---------

Co-authored-by: eric-intuitem <71850047+eric-intuitem@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tools/anssi/anssi-guide-hygiene-detail.xlsx
+++ b/tools/anssi/anssi-guide-hygiene-detail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/anssi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A366A31-B445-274E-B43D-59FB50D9B88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC20E2C1-9D63-FD4A-9521-413BDDC1FECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20580" xr2:uid="{125C4C37-F3C0-444B-A950-381456F8AB10}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="589">
   <si>
     <t>Sensibiliser et former</t>
   </si>
@@ -2074,6 +2074,9 @@
 Vérifier que le référent est responsable de la vérification de l’application des règles.
 Vérifier que le référent est responsable de la sensibilisation des utilisateurs et de la définition d’un plan de formation des acteurs informatiques.
 Vérifier que le référent est responsable de la centralisation et du traitement des incidents de sécurité constatés ou remontés par les utilisateurs.</t>
+  </si>
+  <si>
+    <t>library_publication_date</t>
   </si>
 </sst>
 </file>
@@ -2139,7 +2142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2198,6 +2201,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2533,10 +2539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58679FA1-8C3E-D64B-9B35-083A1517BC84}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="242" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="242" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2558,7 +2564,7 @@
         <v>66</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2571,101 +2577,98 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>112</v>
+        <v>588</v>
+      </c>
+      <c r="B4" s="21">
+        <v>45680</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>407</v>
+        <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>408</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>407</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>110</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2673,31 +2676,42 @@
         <v>79</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>257</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
-    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="3"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2708,9 +2722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F3B91E-FB51-FE47-B7BA-EB94A985CF95}">
   <dimension ref="A1:H260"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="246" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H248" sqref="H248"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3509,6 +3523,9 @@
       </c>
       <c r="B44" s="4">
         <v>3</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
add threats for guide d'hygiène détaillé
</commit_message>
<xml_diff>
--- a/tools/anssi/anssi-guide-hygiene-detail.xlsx
+++ b/tools/anssi/anssi-guide-hygiene-detail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/anssi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC20E2C1-9D63-FD4A-9521-413BDDC1FECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45799CD7-6662-A843-81B7-5DF79DE54F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20580" xr2:uid="{125C4C37-F3C0-444B-A950-381456F8AB10}"/>
+    <workbookView xWindow="5280" yWindow="1200" windowWidth="34560" windowHeight="20240" xr2:uid="{125C4C37-F3C0-444B-A950-381456F8AB10}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="593">
   <si>
     <t>Sensibiliser et former</t>
   </si>
@@ -1352,9 +1352,6 @@
   </si>
   <si>
     <t>library_dependencies</t>
-  </si>
-  <si>
-    <t>urn:intuitem:risk:library:doc-pol</t>
   </si>
   <si>
     <t>En plus des formations générales ci-dessus, vérifier les formations spécifiques suivantes :
@@ -2077,6 +2074,25 @@
   </si>
   <si>
     <t>library_publication_date</t>
+  </si>
+  <si>
+    <t>urn:intuitem:risk:library:doc-pol, urn:intuitem:risk:library:intuitem-common-catalog</t>
+  </si>
+  <si>
+    <t>urn:intuitem:risk:threat:intuitem-common-catalog</t>
+  </si>
+  <si>
+    <t>threat_base_urn</t>
+  </si>
+  <si>
+    <t>threats</t>
+  </si>
+  <si>
+    <t>1:ICT-022
+1:ICT-019
+1:ICT-023
+1:ICT-015
+1:ICT-012</t>
   </si>
 </sst>
 </file>
@@ -2541,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58679FA1-8C3E-D64B-9B35-083A1517BC84}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="242" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2564,7 +2580,7 @@
         <v>66</v>
       </c>
       <c r="B2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2577,7 +2593,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B4" s="21">
         <v>45680</v>
@@ -2636,7 +2652,7 @@
         <v>407</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>408</v>
+        <v>588</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2704,8 +2720,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>590</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
@@ -2720,11 +2744,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F3B91E-FB51-FE47-B7BA-EB94A985CF95}">
-  <dimension ref="A1:H260"/>
+  <dimension ref="A1:I260"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="F1" zoomScale="167" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2736,10 +2760,11 @@
     <col min="6" max="6" width="128.1640625" style="5" customWidth="1"/>
     <col min="7" max="7" width="81.6640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="144" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="5"/>
+    <col min="9" max="9" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>61</v>
       </c>
@@ -2764,8 +2789,11 @@
       <c r="H1" s="5" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="I1" s="5" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="7">
         <v>1</v>
       </c>
@@ -2776,7 +2804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="10">
         <v>2</v>
       </c>
@@ -2792,7 +2820,7 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>63</v>
       </c>
@@ -2809,10 +2837,13 @@
         <v>297</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
@@ -2829,7 +2860,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>63</v>
       </c>
@@ -2846,7 +2877,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
@@ -2863,7 +2894,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>63</v>
       </c>
@@ -2880,7 +2911,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>63</v>
       </c>
@@ -2897,7 +2928,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>63</v>
       </c>
@@ -2914,7 +2945,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>63</v>
       </c>
@@ -2931,7 +2962,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>63</v>
       </c>
@@ -2948,10 +2979,10 @@
         <v>298</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
@@ -2968,10 +2999,10 @@
         <v>258</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B14" s="10">
         <v>2</v>
       </c>
@@ -2987,7 +3018,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>63</v>
       </c>
@@ -3004,10 +3035,10 @@
         <v>299</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
@@ -3024,7 +3055,7 @@
         <v>298</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3095,7 +3126,7 @@
         <v>298</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3115,7 +3146,7 @@
         <v>298</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3169,7 +3200,7 @@
         <v>301</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3201,7 +3232,7 @@
         <v>258</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -3221,7 +3252,7 @@
         <v>258</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3241,7 +3272,7 @@
         <v>302</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3261,7 +3292,7 @@
         <v>303</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3308,7 +3339,7 @@
         <v>304</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="102" x14ac:dyDescent="0.2">
@@ -3328,7 +3359,7 @@
         <v>305</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -3348,7 +3379,7 @@
         <v>306</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3368,7 +3399,7 @@
         <v>306</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -3404,7 +3435,7 @@
         <v>307</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3458,7 +3489,7 @@
         <v>307</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3478,7 +3509,7 @@
         <v>277</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3498,7 +3529,7 @@
         <v>259</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -3534,7 +3565,7 @@
         <v>259</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3554,7 +3585,7 @@
         <v>278</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3574,7 +3605,7 @@
         <v>279</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -3594,7 +3625,7 @@
         <v>260</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3614,7 +3645,7 @@
         <v>261</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3634,7 +3665,7 @@
         <v>305</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3670,7 +3701,7 @@
         <v>262</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3690,7 +3721,7 @@
         <v>263</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3710,7 +3741,7 @@
         <v>262</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3730,7 +3761,7 @@
         <v>319</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3777,7 +3808,7 @@
         <v>259</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -3797,7 +3828,7 @@
         <v>308</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -3817,7 +3848,7 @@
         <v>308</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3873,7 +3904,7 @@
         <v>303</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3893,7 +3924,7 @@
         <v>259</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3913,7 +3944,7 @@
         <v>280</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3933,7 +3964,7 @@
         <v>263</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3953,7 +3984,7 @@
         <v>259</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -3973,7 +4004,7 @@
         <v>262</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3993,7 +4024,7 @@
         <v>277</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -4029,7 +4060,7 @@
         <v>259</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4049,7 +4080,7 @@
         <v>259</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4069,7 +4100,7 @@
         <v>259</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4089,7 +4120,7 @@
         <v>259</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4109,7 +4140,7 @@
         <v>259</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4129,7 +4160,7 @@
         <v>298</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4165,7 +4196,7 @@
         <v>321</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4185,7 +4216,7 @@
         <v>309</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -4221,7 +4252,7 @@
         <v>259</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4239,7 +4270,7 @@
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4259,7 +4290,7 @@
         <v>259</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4295,7 +4326,7 @@
         <v>259</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -4315,7 +4346,7 @@
         <v>259</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="86" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4362,7 +4393,7 @@
         <v>260</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4382,7 +4413,7 @@
         <v>322</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4422,7 +4453,7 @@
         <v>324</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4442,7 +4473,7 @@
         <v>281</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4462,7 +4493,7 @@
         <v>262</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -4482,7 +4513,7 @@
         <v>325</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4518,7 +4549,7 @@
         <v>260</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -4538,7 +4569,7 @@
         <v>326</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4558,7 +4589,7 @@
         <v>326</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4578,7 +4609,7 @@
         <v>282</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="100" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -4614,7 +4645,7 @@
         <v>322</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4650,7 +4681,7 @@
         <v>326</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -4670,7 +4701,7 @@
         <v>326</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -4690,7 +4721,7 @@
         <v>310</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -4710,7 +4741,7 @@
         <v>327</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="107" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4746,7 +4777,7 @@
         <v>346</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -4766,7 +4797,7 @@
         <v>264</v>
       </c>
       <c r="H109" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="110" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4813,7 +4844,7 @@
         <v>262</v>
       </c>
       <c r="H112" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -4833,7 +4864,7 @@
         <v>344</v>
       </c>
       <c r="H113" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4853,7 +4884,7 @@
         <v>328</v>
       </c>
       <c r="H114" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -4889,7 +4920,7 @@
         <v>344</v>
       </c>
       <c r="H116" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -4909,7 +4940,7 @@
         <v>329</v>
       </c>
       <c r="H117" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4929,7 +4960,7 @@
         <v>262</v>
       </c>
       <c r="H118" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4949,7 +4980,7 @@
         <v>262</v>
       </c>
       <c r="H119" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4969,7 +5000,7 @@
         <v>262</v>
       </c>
       <c r="H120" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="121" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4999,13 +5030,13 @@
         <v>85</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>264</v>
       </c>
       <c r="H122" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5041,7 +5072,7 @@
         <v>262</v>
       </c>
       <c r="H124" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -5061,7 +5092,7 @@
         <v>347</v>
       </c>
       <c r="H125" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5079,7 +5110,7 @@
       </c>
       <c r="G126" s="4"/>
       <c r="H126" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5099,7 +5130,7 @@
         <v>265</v>
       </c>
       <c r="H127" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5117,7 +5148,7 @@
       </c>
       <c r="G128" s="4"/>
       <c r="H128" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5137,7 +5168,7 @@
         <v>347</v>
       </c>
       <c r="H129" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5157,7 +5188,7 @@
         <v>330</v>
       </c>
       <c r="H130" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="131" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -5193,7 +5224,7 @@
         <v>311</v>
       </c>
       <c r="H132" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5213,7 +5244,7 @@
         <v>342</v>
       </c>
       <c r="H133" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -5233,7 +5264,7 @@
         <v>343</v>
       </c>
       <c r="H134" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5269,7 +5300,7 @@
         <v>298</v>
       </c>
       <c r="H136" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5289,7 +5320,7 @@
         <v>266</v>
       </c>
       <c r="H137" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5309,7 +5340,7 @@
         <v>263</v>
       </c>
       <c r="H138" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5375,7 +5406,7 @@
         <v>341</v>
       </c>
       <c r="H142" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5395,7 +5426,7 @@
         <v>341</v>
       </c>
       <c r="H143" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -5415,7 +5446,7 @@
         <v>283</v>
       </c>
       <c r="H144" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="145" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5451,7 +5482,7 @@
         <v>330</v>
       </c>
       <c r="H146" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -5471,7 +5502,7 @@
         <v>342</v>
       </c>
       <c r="H147" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5491,7 +5522,7 @@
         <v>342</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5511,7 +5542,7 @@
         <v>331</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5531,7 +5562,7 @@
         <v>284</v>
       </c>
       <c r="H150" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="151" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5567,7 +5598,7 @@
         <v>267</v>
       </c>
       <c r="H152" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5587,7 +5618,7 @@
         <v>267</v>
       </c>
       <c r="H153" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5607,7 +5638,7 @@
         <v>279</v>
       </c>
       <c r="H154" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5627,7 +5658,7 @@
         <v>279</v>
       </c>
       <c r="H155" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="156" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5647,7 +5678,7 @@
         <v>285</v>
       </c>
       <c r="H156" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5667,7 +5698,7 @@
         <v>262</v>
       </c>
       <c r="H157" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="158" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5714,7 +5745,7 @@
         <v>262</v>
       </c>
       <c r="H160" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -5734,7 +5765,7 @@
         <v>349</v>
       </c>
       <c r="H161" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -5754,7 +5785,7 @@
         <v>286</v>
       </c>
       <c r="H162" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="163" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5774,7 +5805,7 @@
         <v>286</v>
       </c>
       <c r="H163" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="164" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5794,7 +5825,7 @@
         <v>286</v>
       </c>
       <c r="H164" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -5830,7 +5861,7 @@
         <v>262</v>
       </c>
       <c r="H166" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="167" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5862,7 +5893,7 @@
         <v>262</v>
       </c>
       <c r="H168" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="169" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -5876,13 +5907,13 @@
         <v>85</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G169" s="4" t="s">
         <v>262</v>
       </c>
       <c r="H169" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5902,7 +5933,7 @@
         <v>262</v>
       </c>
       <c r="H170" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="171" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -5938,7 +5969,7 @@
         <v>260</v>
       </c>
       <c r="H172" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="173" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -5958,7 +5989,7 @@
         <v>312</v>
       </c>
       <c r="H173" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="174" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6005,7 +6036,7 @@
         <v>260</v>
       </c>
       <c r="H176" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -6025,7 +6056,7 @@
         <v>297</v>
       </c>
       <c r="H177" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6045,7 +6076,7 @@
         <v>298</v>
       </c>
       <c r="H178" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6065,7 +6096,7 @@
         <v>332</v>
       </c>
       <c r="H179" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6085,7 +6116,7 @@
         <v>324</v>
       </c>
       <c r="H180" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="181" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -6121,7 +6152,7 @@
         <v>268</v>
       </c>
       <c r="H182" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -6141,7 +6172,7 @@
         <v>333</v>
       </c>
       <c r="H183" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -6161,7 +6192,7 @@
         <v>324</v>
       </c>
       <c r="H184" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="185" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6197,7 +6228,7 @@
         <v>330</v>
       </c>
       <c r="H186" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -6217,7 +6248,7 @@
         <v>334</v>
       </c>
       <c r="H187" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -6237,7 +6268,7 @@
         <v>330</v>
       </c>
       <c r="H188" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -6257,7 +6288,7 @@
         <v>335</v>
       </c>
       <c r="H189" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="190" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6293,7 +6324,7 @@
         <v>269</v>
       </c>
       <c r="H191" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="192" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -6313,7 +6344,7 @@
         <v>322</v>
       </c>
       <c r="H192" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -6350,7 +6381,7 @@
         <v>336</v>
       </c>
       <c r="H194" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="195" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6397,7 +6428,7 @@
         <v>265</v>
       </c>
       <c r="H197" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -6429,7 +6460,7 @@
         <v>286</v>
       </c>
       <c r="H199" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="200" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6449,7 +6480,7 @@
         <v>287</v>
       </c>
       <c r="H200" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="201" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6469,7 +6500,7 @@
         <v>286</v>
       </c>
       <c r="H201" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="202" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -6489,7 +6520,7 @@
         <v>286</v>
       </c>
       <c r="H202" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="203" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -6509,7 +6540,7 @@
         <v>262</v>
       </c>
       <c r="H203" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="204" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -6557,7 +6588,7 @@
         <v>337</v>
       </c>
       <c r="H206" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="207" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -6577,7 +6608,7 @@
         <v>265</v>
       </c>
       <c r="H207" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="208" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -6597,7 +6628,7 @@
         <v>337</v>
       </c>
       <c r="H208" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="209" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -6617,7 +6648,7 @@
         <v>265</v>
       </c>
       <c r="H209" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="210" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6637,7 +6668,7 @@
         <v>313</v>
       </c>
       <c r="H210" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="211" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -6657,7 +6688,7 @@
         <v>258</v>
       </c>
       <c r="H211" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="212" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6677,7 +6708,7 @@
         <v>265</v>
       </c>
       <c r="H212" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="213" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6724,7 +6755,7 @@
         <v>270</v>
       </c>
       <c r="H215" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="216" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6744,7 +6775,7 @@
         <v>314</v>
       </c>
       <c r="H216" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="217" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6764,7 +6795,7 @@
         <v>288</v>
       </c>
       <c r="H217" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="218" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6784,7 +6815,7 @@
         <v>270</v>
       </c>
       <c r="H218" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="219" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -6804,7 +6835,7 @@
         <v>288</v>
       </c>
       <c r="H219" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="220" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -6824,7 +6855,7 @@
         <v>338</v>
       </c>
       <c r="H220" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="221" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -6844,7 +6875,7 @@
         <v>339</v>
       </c>
       <c r="H221" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="222" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -6858,13 +6889,13 @@
         <v>85</v>
       </c>
       <c r="F222" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G222" s="4" t="s">
         <v>339</v>
       </c>
       <c r="H222" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="223" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6884,7 +6915,7 @@
         <v>289</v>
       </c>
       <c r="H223" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="224" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -6904,7 +6935,7 @@
         <v>340</v>
       </c>
       <c r="H224" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="225" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6940,7 +6971,7 @@
         <v>271</v>
       </c>
       <c r="H226" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="227" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -6972,7 +7003,7 @@
         <v>271</v>
       </c>
       <c r="H228" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7106,7 +7137,7 @@
         <v>271</v>
       </c>
       <c r="H236" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="237" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7126,7 +7157,7 @@
         <v>271</v>
       </c>
       <c r="H237" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="238" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7146,7 +7177,7 @@
         <v>272</v>
       </c>
       <c r="H238" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="239" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -7166,7 +7197,7 @@
         <v>272</v>
       </c>
       <c r="H239" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="240" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -7204,7 +7235,7 @@
         <v>273</v>
       </c>
       <c r="H241" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="242" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -7226,7 +7257,7 @@
         <v>315</v>
       </c>
       <c r="H242" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="243" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -7248,7 +7279,7 @@
         <v>316</v>
       </c>
       <c r="H243" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="244" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -7270,7 +7301,7 @@
         <v>274</v>
       </c>
       <c r="H244" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="245" spans="1:8" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -7306,7 +7337,7 @@
         <v>317</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -7326,7 +7357,7 @@
         <v>298</v>
       </c>
       <c r="H247" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="248" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -7346,7 +7377,7 @@
         <v>298</v>
       </c>
       <c r="H248" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="249" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -7366,7 +7397,7 @@
         <v>317</v>
       </c>
       <c r="H249" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="250" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -7402,7 +7433,7 @@
         <v>275</v>
       </c>
       <c r="H251" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="252" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -7422,7 +7453,7 @@
         <v>284</v>
       </c>
       <c r="H252" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="253" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -7442,7 +7473,7 @@
         <v>275</v>
       </c>
       <c r="H253" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="254" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -7462,7 +7493,7 @@
         <v>318</v>
       </c>
       <c r="H254" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="255" spans="1:8" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -7509,7 +7540,7 @@
         <v>276</v>
       </c>
       <c r="H257" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="258" spans="1:8" ht="102" x14ac:dyDescent="0.2">
@@ -7529,7 +7560,7 @@
         <v>273</v>
       </c>
       <c r="H258" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="259" spans="1:8" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -7565,7 +7596,7 @@
         <v>258</v>
       </c>
       <c r="H260" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>